<commit_message>
Basic calculator for farmers Added disclaimer Bugfixes for release builds
</commit_message>
<xml_diff>
--- a/needs.xlsx
+++ b/needs.xlsx
@@ -13,15 +13,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Farmers</t>
   </si>
   <si>
     <t>Houses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Per house</t>
   </si>
   <si>
     <t>Produce</t>
@@ -52,8 +49,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="160" formatCode="0.0000000000"/>
+    <numFmt numFmtId="161" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -90,25 +88,22 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="161" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="9" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="10" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,98 +631,108 @@
     </row>
     <row ht="14.25" r="9">
       <c r="D9" s="1">
-        <v>350</v>
+        <v>800</v>
       </c>
       <c r="E9" s="1">
-        <f>SUM(D9/D10)</f>
-        <v>35</v>
+        <f>SUM(D9*F16)</f>
+        <v>80</v>
       </c>
     </row>
     <row ht="14.25" r="10">
-      <c r="C10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1">
-        <v>10</v>
-      </c>
+      <c r="C10" s="0"/>
+      <c r="D10" s="1"/>
     </row>
     <row ht="14.25" r="11">
       <c r="E11" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="H11" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="I11" s="0" t="s">
+    </row>
+    <row ht="10.5" customHeight="1" r="12">
+      <c r="E12" s="2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row ht="10.5" customHeight="1" r="12">
-      <c r="E12" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row ht="14.25" r="13">
       <c r="D13" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>2.5000002000000001e-003</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="4">
         <f>SUM($D$9*F13)</f>
-        <v>0.87500007000000002</v>
-      </c>
-      <c r="I13" s="6">
+        <v>2.0000001599999999</v>
+      </c>
+      <c r="I13" s="5">
         <f>SUM(H13/E13)</f>
-        <v>0.43750003500000001</v>
+        <v>1.00000008</v>
       </c>
     </row>
     <row ht="14.25" r="14">
       <c r="D14" s="0" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>3.0769259999999998e-003</v>
       </c>
-      <c r="H14" s="5">
-        <f>SUM($D$9*F14)</f>
-        <v>1.0769240999999998</v>
-      </c>
-      <c r="I14" s="6">
-        <f>SUM(H14/E14)</f>
-        <v>0.53846204999999991</v>
+      <c r="H14" s="4">
+        <f ref="H14:H15" si="0" t="shared">SUM($D$9*F14)</f>
+        <v>2.4615407999999999</v>
+      </c>
+      <c r="I14" s="5">
+        <f ref="I14:I15" si="1" t="shared">SUM(H14/E14)</f>
+        <v>1.2307703999999999</v>
       </c>
     </row>
     <row ht="14.25" r="15">
       <c r="D15" s="0" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E15" s="1">
         <v>2</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="3">
         <v>3.3333360000000001e-003</v>
       </c>
-      <c r="H15" s="5">
-        <f>SUM($D$9*F15)</f>
-        <v>1.1666676</v>
-      </c>
-      <c r="I15" s="6">
-        <f>SUM(H15/E15)</f>
-        <v>0.58333380000000001</v>
-      </c>
-    </row>
-    <row ht="14.25" r="16"/>
+      <c r="H15" s="4">
+        <f si="0" t="shared"/>
+        <v>2.6666688000000001</v>
+      </c>
+      <c r="I15" s="5">
+        <f si="1" t="shared"/>
+        <v>1.3333344</v>
+      </c>
+    </row>
+    <row ht="14.25" r="16">
+      <c r="D16" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.10000000000000001</v>
+      </c>
+      <c r="H16" s="4">
+        <f>SUM($D$9*F16)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row ht="14.25" r="19">
+      <c r="H19" s="6"/>
+    </row>
   </sheetData>
   <printOptions headings="0" gridLines="0" gridLinesSet="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.5" footer="0.5"/>

</xml_diff>